<commit_message>
Adding Slow Growth V1 + Trade Balance Indicator
</commit_message>
<xml_diff>
--- a/data processing/Input Files/List_Of_Indicators_GEM.xlsx
+++ b/data processing/Input Files/List_Of_Indicators_GEM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dcrook\Documents\scenario_dashboard\data processing\Input Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7864FFCC-62D6-4EC9-AC39-F1A538A2C1E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF1747B8-D81F-4F9D-8982-4E07C272D764}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0718B14B-BDA5-4677-A130-78AE0681013F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0718B14B-BDA5-4677-A130-78AE0681013F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="198">
   <si>
     <t>Database</t>
   </si>
@@ -621,6 +621,15 @@
   </si>
   <si>
     <t>US$ 2015 prices</t>
+  </si>
+  <si>
+    <t>TRDBAL</t>
+  </si>
+  <si>
+    <t>Trade Balance</t>
+  </si>
+  <si>
+    <t>AUS$</t>
   </si>
 </sst>
 </file>
@@ -995,26 +1004,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3629D064-AF3C-40AE-93DD-210D4C69C1D7}">
-  <dimension ref="A1:H81"/>
+  <dimension ref="A1:H82"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H77" sqref="H77"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F83" sqref="F83"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="1"/>
-    <col min="2" max="2" width="16.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="46.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="16.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="46.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1040,7 +1049,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -1067,7 +1076,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -1094,7 +1103,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -1121,7 +1130,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -1148,7 +1157,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -1175,7 +1184,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
@@ -1202,7 +1211,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>4</v>
       </c>
@@ -1229,7 +1238,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>4</v>
       </c>
@@ -1256,7 +1265,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>4</v>
       </c>
@@ -1283,7 +1292,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>4</v>
       </c>
@@ -1310,7 +1319,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>4</v>
       </c>
@@ -1337,7 +1346,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>4</v>
       </c>
@@ -1364,7 +1373,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>4</v>
       </c>
@@ -1391,7 +1400,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>4</v>
       </c>
@@ -1418,7 +1427,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>4</v>
       </c>
@@ -1445,7 +1454,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>4</v>
       </c>
@@ -1472,7 +1481,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>4</v>
       </c>
@@ -1499,7 +1508,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>4</v>
       </c>
@@ -1526,7 +1535,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>4</v>
       </c>
@@ -1553,7 +1562,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>4</v>
       </c>
@@ -1580,7 +1589,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>4</v>
       </c>
@@ -1607,7 +1616,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>4</v>
       </c>
@@ -1634,7 +1643,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>4</v>
       </c>
@@ -1661,7 +1670,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>4</v>
       </c>
@@ -1688,7 +1697,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>4</v>
       </c>
@@ -1715,7 +1724,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>4</v>
       </c>
@@ -1742,7 +1751,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>4</v>
       </c>
@@ -1769,7 +1778,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>4</v>
       </c>
@@ -1796,7 +1805,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>4</v>
       </c>
@@ -1823,7 +1832,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>4</v>
       </c>
@@ -1850,7 +1859,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>4</v>
       </c>
@@ -1877,7 +1886,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>4</v>
       </c>
@@ -1904,7 +1913,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>4</v>
       </c>
@@ -1931,7 +1940,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>4</v>
       </c>
@@ -1958,7 +1967,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>4</v>
       </c>
@@ -1985,7 +1994,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>4</v>
       </c>
@@ -2012,7 +2021,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>4</v>
       </c>
@@ -2039,7 +2048,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>4</v>
       </c>
@@ -2066,7 +2075,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>4</v>
       </c>
@@ -2093,7 +2102,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>4</v>
       </c>
@@ -2120,7 +2129,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>4</v>
       </c>
@@ -2147,7 +2156,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>4</v>
       </c>
@@ -2174,7 +2183,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>4</v>
       </c>
@@ -2201,7 +2210,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>4</v>
       </c>
@@ -2228,7 +2237,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>4</v>
       </c>
@@ -2255,7 +2264,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>4</v>
       </c>
@@ -2282,7 +2291,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>4</v>
       </c>
@@ -2309,7 +2318,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>4</v>
       </c>
@@ -2336,7 +2345,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>4</v>
       </c>
@@ -2363,7 +2372,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>4</v>
       </c>
@@ -2390,7 +2399,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>4</v>
       </c>
@@ -2417,7 +2426,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>4</v>
       </c>
@@ -2444,7 +2453,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>4</v>
       </c>
@@ -2471,7 +2480,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>4</v>
       </c>
@@ -2498,7 +2507,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>4</v>
       </c>
@@ -2525,7 +2534,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>4</v>
       </c>
@@ -2552,7 +2561,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>4</v>
       </c>
@@ -2579,7 +2588,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>4</v>
       </c>
@@ -2606,7 +2615,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>4</v>
       </c>
@@ -2633,7 +2642,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>4</v>
       </c>
@@ -2660,7 +2669,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>4</v>
       </c>
@@ -2687,7 +2696,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>4</v>
       </c>
@@ -2714,7 +2723,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>4</v>
       </c>
@@ -2741,7 +2750,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>4</v>
       </c>
@@ -2768,7 +2777,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>4</v>
       </c>
@@ -2779,7 +2788,7 @@
         <v>18</v>
       </c>
       <c r="D66" s="1" t="str">
-        <f t="shared" ref="D66:D97" si="2">B66&amp;","&amp;C66</f>
+        <f t="shared" ref="D66:D82" si="2">B66&amp;","&amp;C66</f>
         <v>CPI,AUSTRALI</v>
       </c>
       <c r="E66" s="1" t="s">
@@ -2795,7 +2804,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>4</v>
       </c>
@@ -2822,7 +2831,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>4</v>
       </c>
@@ -2849,7 +2858,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>4</v>
       </c>
@@ -2876,7 +2885,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>4</v>
       </c>
@@ -2903,7 +2912,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>4</v>
       </c>
@@ -2930,7 +2939,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>4</v>
       </c>
@@ -2957,7 +2966,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>4</v>
       </c>
@@ -2984,7 +2993,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>4</v>
       </c>
@@ -3011,7 +3020,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>4</v>
       </c>
@@ -3038,7 +3047,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>4</v>
       </c>
@@ -3065,7 +3074,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>4</v>
       </c>
@@ -3092,7 +3101,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>4</v>
       </c>
@@ -3119,7 +3128,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>4</v>
       </c>
@@ -3146,7 +3155,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>4</v>
       </c>
@@ -3173,7 +3182,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>4</v>
       </c>
@@ -3197,6 +3206,33 @@
         <v>147</v>
       </c>
       <c r="H81" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D82" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>TRDBAL,AUSTRALI</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="G82" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="H82" s="1" t="s">
         <v>187</v>
       </c>
     </row>

</xml_diff>